<commit_message>
feat:gam table file structure created
</commit_message>
<xml_diff>
--- a/tbaadm/sol_group_control_table/sol_group_control_table.xlsx
+++ b/tbaadm/sol_group_control_table/sol_group_control_table.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:NH2"/>
+  <dimension ref="A1:ND2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,2256 +440,2224 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>_airbyte_ab_id</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>_airbyte_emitted_at</t>
+          <t>ts_cnt</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>seed</t>
+          <t>bank_id</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>ts_cnt</t>
+          <t>del_flg</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>bank_id</t>
+          <t>pwd_key</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>del_flg</t>
+          <t>dc_alias</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>pwd_key</t>
+          <t>ft_in_use</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>dc_alias</t>
+          <t>iso_bacid</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>ft_in_use</t>
+          <t>lchg_time</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>iso_bacid</t>
+          <t>minor_age</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>lchg_time</t>
+          <t>rate_code</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>minor_age</t>
+          <t>rcre_time</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>rate_code</t>
+          <t>wkly_off1</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>rcre_time</t>
+          <t>wkly_off2</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>wkly_off1</t>
+          <t>cash_bacid</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>wkly_off2</t>
+          <t>cdci_bacid</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>cash_bacid</t>
+          <t>cdci_solid</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>cdci_bacid</t>
+          <t>dc_cls_flg</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>cdci_solid</t>
+          <t>group_desc</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>dc_cls_flg</t>
+          <t>zakat_pcnt</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>group_desc</t>
+          <t>ack_req_flg</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>zakat_pcnt</t>
+          <t>dc_cls_date</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>ack_req_flg</t>
+          <t>dflt_sol_id</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>dc_cls_date</t>
+          <t>fin_yr_ddmm</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>dflt_sol_id</t>
+          <t>locale_code</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>fin_yr_ddmm</t>
+          <t>mca_enabled</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>locale_code</t>
+          <t>tran_method</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>mca_enabled</t>
+          <t>db_stat_date</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>tran_method</t>
+          <t>dc_stat_code</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>db_stat_date</t>
+          <t>ho_time_zone</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>dc_stat_code</t>
+          <t>lchg_user_id</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>ho_time_zone</t>
+          <t>rcre_user_id</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>lchg_user_id</t>
+          <t>sol_group_id</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>rcre_user_id</t>
+          <t>tc_pur_bacid</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>sol_group_id</t>
+          <t>tds_end_date</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>tc_pur_bacid</t>
+          <t>dp_check_reqd</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>tds_end_date</t>
+          <t>scgl_mcgl_flg</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>dp_check_reqd</t>
+          <t>tax_rate_code</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>scgl_mcgl_flg</t>
+          <t>tc_sale_bacid</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>tax_rate_code</t>
+          <t>tds_scope_flg</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>tc_sale_bacid</t>
+          <t>alt1_lang_code</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
         <is>
-          <t>tds_scope_flg</t>
+          <t>amort_date_flg</t>
         </is>
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>alt1_lang_code</t>
+          <t>base_lang_code</t>
         </is>
       </c>
       <c r="AR1" s="1" t="inlineStr">
         <is>
-          <t>amort_date_flg</t>
+          <t>cdci_rate_code</t>
         </is>
       </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
-          <t>base_lang_code</t>
+          <t>chrg_rate_code</t>
         </is>
       </c>
       <c r="AT1" s="1" t="inlineStr">
         <is>
-          <t>cdci_rate_code</t>
+          <t>dso_job_status</t>
         </is>
       </c>
       <c r="AU1" s="1" t="inlineStr">
         <is>
-          <t>chrg_rate_code</t>
+          <t>fact_rate_code</t>
         </is>
       </c>
       <c r="AV1" s="1" t="inlineStr">
         <is>
-          <t>dso_job_status</t>
+          <t>max_upload_rec</t>
         </is>
       </c>
       <c r="AW1" s="1" t="inlineStr">
         <is>
-          <t>fact_rate_code</t>
+          <t>opconsole_addr</t>
         </is>
       </c>
       <c r="AX1" s="1" t="inlineStr">
         <is>
-          <t>max_upload_rec</t>
+          <t>tds_start_date</t>
         </is>
       </c>
       <c r="AY1" s="1" t="inlineStr">
         <is>
-          <t>opconsole_addr</t>
+          <t>trea_txn_limit</t>
         </is>
       </c>
       <c r="AZ1" s="1" t="inlineStr">
         <is>
-          <t>tds_start_date</t>
+          <t>uniserver_addr</t>
         </is>
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
-          <t>trea_txn_limit</t>
+          <t>use_shadow_bal</t>
         </is>
       </c>
       <c r="BB1" s="1" t="inlineStr">
         <is>
-          <t>uniserver_addr</t>
+          <t>autosuspend_flg</t>
         </is>
       </c>
       <c r="BC1" s="1" t="inlineStr">
         <is>
-          <t>use_shadow_bal</t>
+          <t>batch_oper_date</t>
         </is>
       </c>
       <c r="BD1" s="1" t="inlineStr">
         <is>
-          <t>autosuspend_flg</t>
+          <t>dso_in_progress</t>
         </is>
       </c>
       <c r="BE1" s="1" t="inlineStr">
         <is>
-          <t>batch_oper_date</t>
+          <t>home_cntry_code</t>
         </is>
       </c>
       <c r="BF1" s="1" t="inlineStr">
         <is>
-          <t>dso_in_progress</t>
+          <t>home_crncy_abbr</t>
         </is>
       </c>
       <c r="BG1" s="1" t="inlineStr">
         <is>
-          <t>home_cntry_code</t>
+          <t>home_crncy_code</t>
         </is>
       </c>
       <c r="BH1" s="1" t="inlineStr">
         <is>
-          <t>home_crncy_abbr</t>
+          <t>mud_pool_sol_id</t>
         </is>
       </c>
       <c r="BI1" s="1" t="inlineStr">
         <is>
-          <t>home_crncy_code</t>
+          <t>proxy_post_alwd</t>
         </is>
       </c>
       <c r="BJ1" s="1" t="inlineStr">
         <is>
-          <t>mud_pool_sol_id</t>
+          <t>repay_rate_code</t>
         </is>
       </c>
       <c r="BK1" s="1" t="inlineStr">
         <is>
-          <t>proxy_post_alwd</t>
+          <t>sys_gen_fund_id</t>
         </is>
       </c>
       <c r="BL1" s="1" t="inlineStr">
         <is>
-          <t>repay_rate_code</t>
+          <t>tc_pur_event_id</t>
         </is>
       </c>
       <c r="BM1" s="1" t="inlineStr">
         <is>
-          <t>sys_gen_fund_id</t>
+          <t>tds_implemented</t>
         </is>
       </c>
       <c r="BN1" s="1" t="inlineStr">
         <is>
-          <t>tc_pur_event_id</t>
+          <t>zakat_appl_date</t>
         </is>
       </c>
       <c r="BO1" s="1" t="inlineStr">
         <is>
-          <t>tds_implemented</t>
+          <t>ach_office_bacid</t>
         </is>
       </c>
       <c r="BP1" s="1" t="inlineStr">
         <is>
-          <t>zakat_appl_date</t>
+          <t>dflt_proxy_bacid</t>
         </is>
       </c>
       <c r="BQ1" s="1" t="inlineStr">
         <is>
-          <t>ach_office_bacid</t>
+          <t>la_payment_bacid</t>
         </is>
       </c>
       <c r="BR1" s="1" t="inlineStr">
         <is>
-          <t>dflt_proxy_bacid</t>
+          <t>limit_cont_bacid</t>
         </is>
       </c>
       <c r="BS1" s="1" t="inlineStr">
         <is>
-          <t>la_payment_bacid</t>
+          <t>lm_struct_id_seq</t>
         </is>
       </c>
       <c r="BT1" s="1" t="inlineStr">
         <is>
-          <t>limit_cont_bacid</t>
+          <t>native_lang_code</t>
         </is>
       </c>
       <c r="BU1" s="1" t="inlineStr">
         <is>
-          <t>lm_struct_id_seq</t>
+          <t>pdc_office_bacid</t>
         </is>
       </c>
       <c r="BV1" s="1" t="inlineStr">
         <is>
-          <t>native_lang_code</t>
+          <t>pd_indicator_flg</t>
         </is>
       </c>
       <c r="BW1" s="1" t="inlineStr">
         <is>
-          <t>pdc_office_bacid</t>
+          <t>report_rate_code</t>
         </is>
       </c>
       <c r="BX1" s="1" t="inlineStr">
         <is>
-          <t>pd_indicator_flg</t>
+          <t>send_auth_id_flg</t>
         </is>
       </c>
       <c r="BY1" s="1" t="inlineStr">
         <is>
-          <t>report_rate_code</t>
+          <t>sweeps_rate_code</t>
         </is>
       </c>
       <c r="BZ1" s="1" t="inlineStr">
         <is>
-          <t>send_auth_id_flg</t>
+          <t>syn_contra_bacid</t>
         </is>
       </c>
       <c r="CA1" s="1" t="inlineStr">
         <is>
-          <t>sweeps_rate_code</t>
+          <t>tc_sale_event_id</t>
         </is>
       </c>
       <c r="CB1" s="1" t="inlineStr">
         <is>
-          <t>syn_contra_bacid</t>
+          <t>adhoc_cs_event_id</t>
         </is>
       </c>
       <c r="CC1" s="1" t="inlineStr">
         <is>
-          <t>tc_sale_event_id</t>
+          <t>asset_id_sequence</t>
         </is>
       </c>
       <c r="CD1" s="1" t="inlineStr">
         <is>
-          <t>adhoc_cs_event_id</t>
+          <t>bancsconnect_addr</t>
         </is>
       </c>
       <c r="CE1" s="1" t="inlineStr">
         <is>
-          <t>asset_id_sequence</t>
+          <t>cdci_stlmnt_bacid</t>
         </is>
       </c>
       <c r="CF1" s="1" t="inlineStr">
         <is>
-          <t>bancsconnect_addr</t>
+          <t>cdci_stlmnt_solid</t>
         </is>
       </c>
       <c r="CG1" s="1" t="inlineStr">
         <is>
-          <t>cdci_stlmnt_bacid</t>
+          <t>central_bank_code</t>
         </is>
       </c>
       <c r="CH1" s="1" t="inlineStr">
         <is>
-          <t>cdci_stlmnt_solid</t>
+          <t>crystal_rate_code</t>
         </is>
       </c>
       <c r="CI1" s="1" t="inlineStr">
         <is>
-          <t>central_bank_code</t>
+          <t>denom_req_chk_flg</t>
         </is>
       </c>
       <c r="CJ1" s="1" t="inlineStr">
         <is>
-          <t>crystal_rate_code</t>
+          <t>inq_chrgs_enabled</t>
         </is>
       </c>
       <c r="CK1" s="1" t="inlineStr">
         <is>
-          <t>denom_req_chk_flg</t>
+          <t>iso_tran_cre_mode</t>
         </is>
       </c>
       <c r="CL1" s="1" t="inlineStr">
         <is>
-          <t>inq_chrgs_enabled</t>
+          <t>lm_back_value_swp</t>
         </is>
       </c>
       <c r="CM1" s="1" t="inlineStr">
         <is>
-          <t>iso_tran_cre_mode</t>
+          <t>mca_auto_cls_days</t>
         </is>
       </c>
       <c r="CN1" s="1" t="inlineStr">
         <is>
-          <t>lm_back_value_swp</t>
+          <t>new_acct_duration</t>
         </is>
       </c>
       <c r="CO1" s="1" t="inlineStr">
         <is>
-          <t>mca_auto_cls_days</t>
+          <t>next_fund_id_code</t>
         </is>
       </c>
       <c r="CP1" s="1" t="inlineStr">
         <is>
-          <t>new_acct_duration</t>
+          <t>part_tran_vfd_flg</t>
         </is>
       </c>
       <c r="CQ1" s="1" t="inlineStr">
         <is>
-          <t>next_fund_id_code</t>
+          <t>pos_tran_event_id</t>
         </is>
       </c>
       <c r="CR1" s="1" t="inlineStr">
         <is>
-          <t>part_tran_vfd_flg</t>
+          <t>sync_despatch_flg</t>
         </is>
       </c>
       <c r="CS1" s="1" t="inlineStr">
         <is>
-          <t>pos_tran_event_id</t>
+          <t>syn_parking_bacid</t>
         </is>
       </c>
       <c r="CT1" s="1" t="inlineStr">
         <is>
-          <t>sync_despatch_flg</t>
+          <t>acct_type_sequence</t>
         </is>
       </c>
       <c r="CU1" s="1" t="inlineStr">
         <is>
-          <t>syn_parking_bacid</t>
+          <t>ach_value_date_flg</t>
         </is>
       </c>
       <c r="CV1" s="1" t="inlineStr">
         <is>
-          <t>acct_type_sequence</t>
+          <t>cdci_payment_bacid</t>
         </is>
       </c>
       <c r="CW1" s="1" t="inlineStr">
         <is>
-          <t>ach_value_date_flg</t>
+          <t>cdci_payment_solid</t>
         </is>
       </c>
       <c r="CX1" s="1" t="inlineStr">
         <is>
-          <t>cdci_payment_bacid</t>
+          <t>clg_suspense_bacid</t>
         </is>
       </c>
       <c r="CY1" s="1" t="inlineStr">
         <is>
-          <t>cdci_payment_solid</t>
+          <t>cons_bal_rate_code</t>
         </is>
       </c>
       <c r="CZ1" s="1" t="inlineStr">
         <is>
-          <t>clg_suspense_bacid</t>
+          <t>cre_limit_tran_flg</t>
         </is>
       </c>
       <c r="DA1" s="1" t="inlineStr">
         <is>
-          <t>cons_bal_rate_code</t>
+          <t>cust_prov_cr_bacid</t>
         </is>
       </c>
       <c r="DB1" s="1" t="inlineStr">
         <is>
-          <t>cre_limit_tran_flg</t>
+          <t>cust_prov_dr_bacid</t>
         </is>
       </c>
       <c r="DC1" s="1" t="inlineStr">
         <is>
-          <t>cust_prov_cr_bacid</t>
+          <t>dealer_id_sequence</t>
         </is>
       </c>
       <c r="DD1" s="1" t="inlineStr">
         <is>
-          <t>cust_prov_dr_bacid</t>
+          <t>disburse_rate_code</t>
         </is>
       </c>
       <c r="DE1" s="1" t="inlineStr">
         <is>
-          <t>dealer_id_sequence</t>
+          <t>linked_entity_excp</t>
         </is>
       </c>
       <c r="DF1" s="1" t="inlineStr">
         <is>
-          <t>disburse_rate_code</t>
+          <t>local_override_flg</t>
         </is>
       </c>
       <c r="DG1" s="1" t="inlineStr">
         <is>
-          <t>linked_entity_excp</t>
+          <t>mca_auto_cls_mnths</t>
         </is>
       </c>
       <c r="DH1" s="1" t="inlineStr">
         <is>
-          <t>local_override_flg</t>
+          <t>npa_prov_rate_code</t>
         </is>
       </c>
       <c r="DI1" s="1" t="inlineStr">
         <is>
-          <t>mca_auto_cls_mnths</t>
+          <t>opconsole_port_nbr</t>
         </is>
       </c>
       <c r="DJ1" s="1" t="inlineStr">
         <is>
-          <t>npa_prov_rate_code</t>
+          <t>pop_cs_details_flg</t>
         </is>
       </c>
       <c r="DK1" s="1" t="inlineStr">
         <is>
-          <t>opconsole_port_nbr</t>
+          <t>pw_validity_period</t>
         </is>
       </c>
       <c r="DL1" s="1" t="inlineStr">
         <is>
-          <t>pop_cs_details_flg</t>
+          <t>td_repay_rate_code</t>
         </is>
       </c>
       <c r="DM1" s="1" t="inlineStr">
         <is>
-          <t>pw_validity_period</t>
+          <t>time_based_eod_flg</t>
         </is>
       </c>
       <c r="DN1" s="1" t="inlineStr">
         <is>
-          <t>td_repay_rate_code</t>
+          <t>uniserver_port_nbr</t>
         </is>
       </c>
       <c r="DO1" s="1" t="inlineStr">
         <is>
-          <t>time_based_eod_flg</t>
+          <t>zakat_ded_cal_base</t>
         </is>
       </c>
       <c r="DP1" s="1" t="inlineStr">
         <is>
-          <t>uniserver_port_nbr</t>
+          <t>additional_cal_base</t>
         </is>
       </c>
       <c r="DQ1" s="1" t="inlineStr">
         <is>
-          <t>zakat_ded_cal_base</t>
+          <t>address_id_sequence</t>
         </is>
       </c>
       <c r="DR1" s="1" t="inlineStr">
         <is>
-          <t>additional_cal_base</t>
+          <t>asset_code_sequence</t>
         </is>
       </c>
       <c r="DS1" s="1" t="inlineStr">
         <is>
-          <t>address_id_sequence</t>
+          <t>bg_sys_cre_tran_flg</t>
         </is>
       </c>
       <c r="DT1" s="1" t="inlineStr">
         <is>
-          <t>asset_code_sequence</t>
+          <t>cdci_suspense_bacid</t>
         </is>
       </c>
       <c r="DU1" s="1" t="inlineStr">
         <is>
-          <t>bg_sys_cre_tran_flg</t>
+          <t>cdci_suspense_solid</t>
         </is>
       </c>
       <c r="DV1" s="1" t="inlineStr">
         <is>
-          <t>cdci_suspense_bacid</t>
+          <t>cond_precedent_excp</t>
         </is>
       </c>
       <c r="DW1" s="1" t="inlineStr">
         <is>
-          <t>cdci_suspense_solid</t>
+          <t>cont_reval_reqd_flg</t>
         </is>
       </c>
       <c r="DX1" s="1" t="inlineStr">
         <is>
-          <t>cond_precedent_excp</t>
+          <t>csis_repl_serv_addr</t>
         </is>
       </c>
       <c r="DY1" s="1" t="inlineStr">
         <is>
-          <t>cont_reval_reqd_flg</t>
+          <t>cust_prov_rate_code</t>
         </is>
       </c>
       <c r="DZ1" s="1" t="inlineStr">
         <is>
-          <t>csis_repl_serv_addr</t>
+          <t>fwc_pl_income_bacid</t>
         </is>
       </c>
       <c r="EA1" s="1" t="inlineStr">
         <is>
-          <t>cust_prov_rate_code</t>
+          <t>fwd_pl_income_bacid</t>
         </is>
       </c>
       <c r="EB1" s="1" t="inlineStr">
         <is>
-          <t>fwc_pl_income_bacid</t>
+          <t>lim_expiry_comp_flg</t>
         </is>
       </c>
       <c r="EC1" s="1" t="inlineStr">
         <is>
-          <t>fwd_pl_income_bacid</t>
+          <t>next_mca_num_prefix</t>
         </is>
       </c>
       <c r="ED1" s="1" t="inlineStr">
         <is>
-          <t>lim_expiry_comp_flg</t>
+          <t>num_of_days_for_pr5</t>
         </is>
       </c>
       <c r="EE1" s="1" t="inlineStr">
         <is>
-          <t>next_mca_num_prefix</t>
+          <t>num_of_days_for_pr6</t>
         </is>
       </c>
       <c r="EF1" s="1" t="inlineStr">
         <is>
-          <t>num_of_days_for_pr5</t>
+          <t>payment_enabled_flg</t>
         </is>
       </c>
       <c r="EG1" s="1" t="inlineStr">
         <is>
-          <t>num_of_days_for_pr6</t>
+          <t>pend_swift_msg_excp</t>
         </is>
       </c>
       <c r="EH1" s="1" t="inlineStr">
         <is>
-          <t>payment_enabled_flg</t>
+          <t>processing_cal_base</t>
         </is>
       </c>
       <c r="EI1" s="1" t="inlineStr">
         <is>
-          <t>pend_swift_msg_excp</t>
+          <t>recog_int_as_income</t>
         </is>
       </c>
       <c r="EJ1" s="1" t="inlineStr">
         <is>
-          <t>processing_cal_base</t>
+          <t>regular_cs_event_id</t>
         </is>
       </c>
       <c r="EK1" s="1" t="inlineStr">
         <is>
-          <t>recog_int_as_income</t>
+          <t>si_history_reqd_flg</t>
         </is>
       </c>
       <c r="EL1" s="1" t="inlineStr">
         <is>
-          <t>regular_cs_event_id</t>
+          <t>sys_gen_cust_id_flg</t>
         </is>
       </c>
       <c r="EM1" s="1" t="inlineStr">
         <is>
-          <t>si_history_reqd_flg</t>
+          <t>td_regflow_with_tds</t>
         </is>
       </c>
       <c r="EN1" s="1" t="inlineStr">
         <is>
-          <t>sys_gen_cust_id_flg</t>
+          <t>use_sundry_acct_flg</t>
         </is>
       </c>
       <c r="EO1" s="1" t="inlineStr">
         <is>
-          <t>td_regflow_with_tds</t>
+          <t>zakat_parking_bacid</t>
         </is>
       </c>
       <c r="EP1" s="1" t="inlineStr">
         <is>
-          <t>use_sundry_acct_flg</t>
+          <t>zakat_threshold_amt</t>
         </is>
       </c>
       <c r="EQ1" s="1" t="inlineStr">
         <is>
-          <t>zakat_parking_bacid</t>
+          <t>acct_cls_reason_code</t>
         </is>
       </c>
       <c r="ER1" s="1" t="inlineStr">
         <is>
-          <t>zakat_threshold_amt</t>
+          <t>auth_submit_reqd_flg</t>
         </is>
       </c>
       <c r="ES1" s="1" t="inlineStr">
         <is>
-          <t>acct_cls_reason_code</t>
+          <t>auto_acct_status_upd</t>
         </is>
       </c>
       <c r="ET1" s="1" t="inlineStr">
         <is>
-          <t>auth_submit_reqd_flg</t>
+          <t>bank_limit_excp_code</t>
         </is>
       </c>
       <c r="EU1" s="1" t="inlineStr">
         <is>
-          <t>auto_acct_status_upd</t>
+          <t>bjms_implemented_flg</t>
         </is>
       </c>
       <c r="EV1" s="1" t="inlineStr">
         <is>
-          <t>bank_limit_excp_code</t>
+          <t>ccy_cal_implmntd_flg</t>
         </is>
       </c>
       <c r="EW1" s="1" t="inlineStr">
         <is>
-          <t>bjms_implemented_flg</t>
+          <t>cdci_tran_back_dated</t>
         </is>
       </c>
       <c r="EX1" s="1" t="inlineStr">
         <is>
-          <t>ccy_cal_implmntd_flg</t>
+          <t>cooperative_bank_flg</t>
         </is>
       </c>
       <c r="EY1" s="1" t="inlineStr">
         <is>
-          <t>cdci_tran_back_dated</t>
+          <t>cust_prov_crncy_code</t>
         </is>
       </c>
       <c r="EZ1" s="1" t="inlineStr">
         <is>
-          <t>cooperative_bank_flg</t>
+          <t>dflt_sub_asset_class</t>
         </is>
       </c>
       <c r="FA1" s="1" t="inlineStr">
         <is>
-          <t>cust_prov_crncy_code</t>
+          <t>iban_implemented_flg</t>
         </is>
       </c>
       <c r="FB1" s="1" t="inlineStr">
         <is>
-          <t>dflt_sub_asset_class</t>
+          <t>ignore_ci_in_closure</t>
         </is>
       </c>
       <c r="FC1" s="1" t="inlineStr">
         <is>
-          <t>iban_implemented_flg</t>
+          <t>implemented_24x7_flg</t>
         </is>
       </c>
       <c r="FD1" s="1" t="inlineStr">
         <is>
-          <t>ignore_ci_in_closure</t>
+          <t>limit_conv_rate_code</t>
         </is>
       </c>
       <c r="FE1" s="1" t="inlineStr">
         <is>
-          <t>implemented_24x7_flg</t>
+          <t>master_auto_cls_days</t>
         </is>
       </c>
       <c r="FF1" s="1" t="inlineStr">
         <is>
-          <t>limit_conv_rate_code</t>
+          <t>max_clerk_work_class</t>
         </is>
       </c>
       <c r="FG1" s="1" t="inlineStr">
         <is>
-          <t>master_auto_cls_days</t>
+          <t>max_firc_agnst_remit</t>
         </is>
       </c>
       <c r="FH1" s="1" t="inlineStr">
         <is>
-          <t>max_clerk_work_class</t>
+          <t>next_zakat_coll_date</t>
         </is>
       </c>
       <c r="FI1" s="1" t="inlineStr">
         <is>
-          <t>max_firc_agnst_remit</t>
+          <t>pay_profit_for_hldys</t>
         </is>
       </c>
       <c r="FJ1" s="1" t="inlineStr">
         <is>
-          <t>next_zakat_coll_date</t>
+          <t>profit_booking_level</t>
         </is>
       </c>
       <c r="FK1" s="1" t="inlineStr">
         <is>
-          <t>pay_profit_for_hldys</t>
+          <t>referral_enabled_flg</t>
         </is>
       </c>
       <c r="FL1" s="1" t="inlineStr">
         <is>
-          <t>profit_booking_level</t>
+          <t>ref_appr_lmt_chk_flg</t>
         </is>
       </c>
       <c r="FM1" s="1" t="inlineStr">
         <is>
-          <t>referral_enabled_flg</t>
+          <t>round_off_booked_amt</t>
         </is>
       </c>
       <c r="FN1" s="1" t="inlineStr">
         <is>
-          <t>ref_appr_lmt_chk_flg</t>
+          <t>short_suspense_bacid</t>
         </is>
       </c>
       <c r="FO1" s="1" t="inlineStr">
         <is>
-          <t>round_off_booked_amt</t>
+          <t>sis_in_operation_flg</t>
         </is>
       </c>
       <c r="FP1" s="1" t="inlineStr">
         <is>
-          <t>short_suspense_bacid</t>
+          <t>si_dr_acct_excp_code</t>
         </is>
       </c>
       <c r="FQ1" s="1" t="inlineStr">
         <is>
-          <t>sis_in_operation_flg</t>
+          <t>syst_gen_mca_num_flg</t>
         </is>
       </c>
       <c r="FR1" s="1" t="inlineStr">
         <is>
-          <t>si_dr_acct_excp_code</t>
+          <t>trea_txn_limit_crncy</t>
         </is>
       </c>
       <c r="FS1" s="1" t="inlineStr">
         <is>
-          <t>syst_gen_mca_num_flg</t>
+          <t>unprntd_ba_excp_code</t>
         </is>
       </c>
       <c r="FT1" s="1" t="inlineStr">
         <is>
-          <t>trea_txn_limit_crncy</t>
+          <t>unvrfd_hot_excp_code</t>
         </is>
       </c>
       <c r="FU1" s="1" t="inlineStr">
         <is>
-          <t>unprntd_ba_excp_code</t>
+          <t>bancsconnect_port_nbr</t>
         </is>
       </c>
       <c r="FV1" s="1" t="inlineStr">
         <is>
-          <t>unvrfd_hot_excp_code</t>
+          <t>buyer_limit_excp_code</t>
         </is>
       </c>
       <c r="FW1" s="1" t="inlineStr">
         <is>
-          <t>bancsconnect_port_nbr</t>
+          <t>ccy_hol_treatment_flg</t>
         </is>
       </c>
       <c r="FX1" s="1" t="inlineStr">
         <is>
-          <t>buyer_limit_excp_code</t>
+          <t>cdci_operating_status</t>
         </is>
       </c>
       <c r="FY1" s="1" t="inlineStr">
         <is>
-          <t>ccy_hol_treatment_flg</t>
+          <t>chq_book_ack_reqd_flg</t>
         </is>
       </c>
       <c r="FZ1" s="1" t="inlineStr">
         <is>
-          <t>cdci_operating_status</t>
+          <t>cmdty_limit_excp_code</t>
         </is>
       </c>
       <c r="GA1" s="1" t="inlineStr">
         <is>
-          <t>chq_book_ack_reqd_flg</t>
+          <t>cntry_limit_excp_code</t>
         </is>
       </c>
       <c r="GB1" s="1" t="inlineStr">
         <is>
-          <t>cmdty_limit_excp_code</t>
+          <t>coll_flow_id_for_cust</t>
         </is>
       </c>
       <c r="GC1" s="1" t="inlineStr">
         <is>
-          <t>cntry_limit_excp_code</t>
+          <t>crncy_limit_excp_code</t>
         </is>
       </c>
       <c r="GD1" s="1" t="inlineStr">
         <is>
-          <t>coll_flow_id_for_cust</t>
+          <t>dc_restartability_flg</t>
         </is>
       </c>
       <c r="GE1" s="1" t="inlineStr">
         <is>
-          <t>crncy_limit_excp_code</t>
+          <t>depo_lien_adj_req_flg</t>
         </is>
       </c>
       <c r="GF1" s="1" t="inlineStr">
         <is>
-          <t>dc_restartability_flg</t>
+          <t>dflt_main_asset_class</t>
         </is>
       </c>
       <c r="GG1" s="1" t="inlineStr">
         <is>
-          <t>depo_lien_adj_req_flg</t>
+          <t>dorm_applicable_to_td</t>
         </is>
       </c>
       <c r="GH1" s="1" t="inlineStr">
         <is>
-          <t>dflt_main_asset_class</t>
+          <t>encrypt_email_reports</t>
         </is>
       </c>
       <c r="GI1" s="1" t="inlineStr">
         <is>
-          <t>dorm_applicable_to_td</t>
+          <t>excess_suspense_bacid</t>
         </is>
       </c>
       <c r="GJ1" s="1" t="inlineStr">
         <is>
-          <t>encrypt_email_reports</t>
+          <t>interest_avail_for_td</t>
         </is>
       </c>
       <c r="GK1" s="1" t="inlineStr">
         <is>
-          <t>excess_suspense_bacid</t>
+          <t>interest_rate_code_cr</t>
         </is>
       </c>
       <c r="GL1" s="1" t="inlineStr">
         <is>
-          <t>interest_avail_for_td</t>
+          <t>interest_rate_code_dr</t>
         </is>
       </c>
       <c r="GM1" s="1" t="inlineStr">
         <is>
-          <t>interest_rate_code_cr</t>
+          <t>last_local_cal_update</t>
         </is>
       </c>
       <c r="GN1" s="1" t="inlineStr">
         <is>
-          <t>interest_rate_code_dr</t>
+          <t>last_pbf_extr_seq_num</t>
         </is>
       </c>
       <c r="GO1" s="1" t="inlineStr">
         <is>
-          <t>last_local_cal_update</t>
+          <t>limit_cont_liab_bacid</t>
         </is>
       </c>
       <c r="GP1" s="1" t="inlineStr">
         <is>
-          <t>last_pbf_extr_seq_num</t>
+          <t>master_auto_cls_mnths</t>
         </is>
       </c>
       <c r="GQ1" s="1" t="inlineStr">
         <is>
-          <t>limit_cont_liab_bacid</t>
+          <t>si_exec_not_completed</t>
         </is>
       </c>
       <c r="GR1" s="1" t="inlineStr">
         <is>
-          <t>master_auto_cls_mnths</t>
+          <t>sweep_schm_type_order</t>
         </is>
       </c>
       <c r="GS1" s="1" t="inlineStr">
         <is>
-          <t>si_exec_not_completed</t>
+          <t>sys_gen_insurance_num</t>
         </is>
       </c>
       <c r="GT1" s="1" t="inlineStr">
         <is>
-          <t>sweep_schm_type_order</t>
+          <t>td_calc_int_for_hldys</t>
         </is>
       </c>
       <c r="GU1" s="1" t="inlineStr">
         <is>
-          <t>sys_gen_insurance_num</t>
+          <t>acct_turnover_perd_ind</t>
         </is>
       </c>
       <c r="GV1" s="1" t="inlineStr">
         <is>
-          <t>td_calc_int_for_hldys</t>
+          <t>cdci_num_of_mini_stmnt</t>
         </is>
       </c>
       <c r="GW1" s="1" t="inlineStr">
         <is>
-          <t>acct_turnover_perd_ind</t>
+          <t>coltrl_reval_rate_code</t>
         </is>
       </c>
       <c r="GX1" s="1" t="inlineStr">
         <is>
-          <t>cdci_num_of_mini_stmnt</t>
+          <t>def_num_of_days_in_mth</t>
         </is>
       </c>
       <c r="GY1" s="1" t="inlineStr">
         <is>
-          <t>coltrl_reval_rate_code</t>
+          <t>ffd_no_break_on_minbal</t>
         </is>
       </c>
       <c r="GZ1" s="1" t="inlineStr">
         <is>
-          <t>def_num_of_days_in_mth</t>
+          <t>future_value_dt_cr_flg</t>
         </is>
       </c>
       <c r="HA1" s="1" t="inlineStr">
         <is>
-          <t>ffd_no_break_on_minbal</t>
+          <t>future_value_dt_dr_flg</t>
         </is>
       </c>
       <c r="HB1" s="1" t="inlineStr">
         <is>
-          <t>future_value_dt_cr_flg</t>
+          <t>fwc_pl_provision_bacid</t>
         </is>
       </c>
       <c r="HC1" s="1" t="inlineStr">
         <is>
-          <t>future_value_dt_dr_flg</t>
+          <t>fwd_pl_provision_bacid</t>
         </is>
       </c>
       <c r="HD1" s="1" t="inlineStr">
         <is>
-          <t>fwc_pl_provision_bacid</t>
+          <t>home_crncy_exchg_bacid</t>
         </is>
       </c>
       <c r="HE1" s="1" t="inlineStr">
         <is>
-          <t>fwd_pl_provision_bacid</t>
+          <t>instrmnt_hot_excp_code</t>
         </is>
       </c>
       <c r="HF1" s="1" t="inlineStr">
         <is>
-          <t>home_crncy_exchg_bacid</t>
+          <t>intcalc_for_regul_tods</t>
         </is>
       </c>
       <c r="HG1" s="1" t="inlineStr">
         <is>
-          <t>instrmnt_hot_excp_code</t>
+          <t>inw_clg_zone_open_excp</t>
         </is>
       </c>
       <c r="HH1" s="1" t="inlineStr">
         <is>
-          <t>intcalc_for_regul_tods</t>
+          <t>loan_acct_cr_excp_code</t>
         </is>
       </c>
       <c r="HI1" s="1" t="inlineStr">
         <is>
-          <t>inw_clg_zone_open_excp</t>
+          <t>max_num_of_lines_in_pb</t>
         </is>
       </c>
       <c r="HJ1" s="1" t="inlineStr">
         <is>
-          <t>loan_acct_cr_excp_code</t>
+          <t>max_sal_loan_lien_pcnt</t>
         </is>
       </c>
       <c r="HK1" s="1" t="inlineStr">
         <is>
-          <t>max_num_of_lines_in_pb</t>
+          <t>num_of_lines_per_folio</t>
         </is>
       </c>
       <c r="HL1" s="1" t="inlineStr">
         <is>
-          <t>max_sal_loan_lien_pcnt</t>
+          <t>oper_on_lien_acct_excp</t>
         </is>
       </c>
       <c r="HM1" s="1" t="inlineStr">
         <is>
-          <t>num_of_lines_per_folio</t>
+          <t>out_clg_zone_open_excp</t>
         </is>
       </c>
       <c r="HN1" s="1" t="inlineStr">
         <is>
-          <t>oper_on_lien_acct_excp</t>
+          <t>pending_auth_excp_code</t>
         </is>
       </c>
       <c r="HO1" s="1" t="inlineStr">
         <is>
-          <t>out_clg_zone_open_excp</t>
+          <t>pending_bars_excp_code</t>
         </is>
       </c>
       <c r="HP1" s="1" t="inlineStr">
         <is>
-          <t>pending_auth_excp_code</t>
+          <t>sys_lien_mod_excp_code</t>
         </is>
       </c>
       <c r="HQ1" s="1" t="inlineStr">
         <is>
-          <t>pending_bars_excp_code</t>
+          <t>td_366_base_in_leap_yr</t>
         </is>
       </c>
       <c r="HR1" s="1" t="inlineStr">
         <is>
-          <t>sys_lien_mod_excp_code</t>
+          <t>td_shift_maturity_date</t>
         </is>
       </c>
       <c r="HS1" s="1" t="inlineStr">
         <is>
-          <t>td_366_base_in_leap_yr</t>
+          <t>tran_not_vfd_excp_code</t>
         </is>
       </c>
       <c r="HT1" s="1" t="inlineStr">
         <is>
-          <t>td_shift_maturity_date</t>
+          <t>unprntd_bars_excp_code</t>
         </is>
       </c>
       <c r="HU1" s="1" t="inlineStr">
         <is>
-          <t>tran_not_vfd_excp_code</t>
+          <t>usr_lim_home_crncy_flg</t>
         </is>
       </c>
       <c r="HV1" s="1" t="inlineStr">
         <is>
-          <t>unprntd_bars_excp_code</t>
+          <t>acct_cust_mismatch_excp</t>
         </is>
       </c>
       <c r="HW1" s="1" t="inlineStr">
         <is>
-          <t>usr_lim_home_crncy_flg</t>
+          <t>bar_gen_not_regularised</t>
         </is>
       </c>
       <c r="HX1" s="1" t="inlineStr">
         <is>
-          <t>acct_cust_mismatch_excp</t>
+          <t>csis_repl_serv_port_nbr</t>
         </is>
       </c>
       <c r="HY1" s="1" t="inlineStr">
         <is>
-          <t>bar_gen_not_regularised</t>
+          <t>cust_accts_inq_event_id</t>
         </is>
       </c>
       <c r="HZ1" s="1" t="inlineStr">
         <is>
-          <t>csis_repl_serv_port_nbr</t>
+          <t>dflt_tod_chng_excp_code</t>
         </is>
       </c>
       <c r="IA1" s="1" t="inlineStr">
         <is>
-          <t>cust_accts_inq_event_id</t>
+          <t>gst_based_on_val_dt_flg</t>
         </is>
       </c>
       <c r="IB1" s="1" t="inlineStr">
         <is>
-          <t>dflt_tod_chng_excp_code</t>
+          <t>iso_bal_check_excp_code</t>
         </is>
       </c>
       <c r="IC1" s="1" t="inlineStr">
         <is>
-          <t>gst_based_on_val_dt_flg</t>
+          <t>last_pbf_extr_date_time</t>
         </is>
       </c>
       <c r="ID1" s="1" t="inlineStr">
         <is>
-          <t>iso_bal_check_excp_code</t>
+          <t>next_insurance_num_code</t>
         </is>
       </c>
       <c r="IE1" s="1" t="inlineStr">
         <is>
-          <t>last_pbf_extr_date_time</t>
+          <t>non_perf_cust_excp_code</t>
         </is>
       </c>
       <c r="IF1" s="1" t="inlineStr">
         <is>
-          <t>next_insurance_num_code</t>
+          <t>pdc_zone_value_date_flg</t>
         </is>
       </c>
       <c r="IG1" s="1" t="inlineStr">
         <is>
-          <t>non_perf_cust_excp_code</t>
+          <t>pur_sale_pend_excp_code</t>
         </is>
       </c>
       <c r="IH1" s="1" t="inlineStr">
         <is>
-          <t>pdc_zone_value_date_flg</t>
+          <t>raise_sales_trigger_ind</t>
         </is>
       </c>
       <c r="II1" s="1" t="inlineStr">
         <is>
-          <t>pur_sale_pend_excp_code</t>
+          <t>td_cls_calc_overdue_int</t>
         </is>
       </c>
       <c r="IJ1" s="1" t="inlineStr">
         <is>
-          <t>raise_sales_trigger_ind</t>
+          <t>td_drp_acct_balance_chk</t>
         </is>
       </c>
       <c r="IK1" s="1" t="inlineStr">
         <is>
-          <t>td_cls_calc_overdue_int</t>
+          <t>td_drp_after_auto_renew</t>
         </is>
       </c>
       <c r="IL1" s="1" t="inlineStr">
         <is>
-          <t>td_drp_acct_balance_chk</t>
+          <t>tran_not_pstd_excp_code</t>
         </is>
       </c>
       <c r="IM1" s="1" t="inlineStr">
         <is>
-          <t>td_drp_after_auto_renew</t>
+          <t>tran_not_stop_excp_code</t>
         </is>
       </c>
       <c r="IN1" s="1" t="inlineStr">
         <is>
-          <t>tran_not_pstd_excp_code</t>
+          <t>upfront_cont_limit_reqd</t>
         </is>
       </c>
       <c r="IO1" s="1" t="inlineStr">
         <is>
-          <t>tran_not_stop_excp_code</t>
+          <t>use_prev_data_for_accrl</t>
         </is>
       </c>
       <c r="IP1" s="1" t="inlineStr">
         <is>
-          <t>upfront_cont_limit_reqd</t>
+          <t>back_value_dated_inw_clg</t>
         </is>
       </c>
       <c r="IQ1" s="1" t="inlineStr">
         <is>
-          <t>use_prev_data_for_accrl</t>
+          <t>capture_clrng_instr_dtls</t>
         </is>
       </c>
       <c r="IR1" s="1" t="inlineStr">
         <is>
-          <t>back_value_dated_inw_clg</t>
+          <t>ddall_not_prnt_excp_code</t>
         </is>
       </c>
       <c r="IS1" s="1" t="inlineStr">
         <is>
-          <t>capture_clrng_instr_dtls</t>
+          <t>df_ch_not_adst_excp_code</t>
         </is>
       </c>
       <c r="IT1" s="1" t="inlineStr">
         <is>
-          <t>ddall_not_prnt_excp_code</t>
+          <t>due_on_holiday_excp_code</t>
         </is>
       </c>
       <c r="IU1" s="1" t="inlineStr">
         <is>
-          <t>df_ch_not_adst_excp_code</t>
+          <t>dummy_acct_bal_excp_code</t>
         </is>
       </c>
       <c r="IV1" s="1" t="inlineStr">
         <is>
-          <t>due_on_holiday_excp_code</t>
+          <t>fc_vault_conv_crncy_code</t>
         </is>
       </c>
       <c r="IW1" s="1" t="inlineStr">
         <is>
-          <t>dummy_acct_bal_excp_code</t>
+          <t>fi_payment_tran_event_id</t>
         </is>
       </c>
       <c r="IX1" s="1" t="inlineStr">
         <is>
-          <t>fc_vault_conv_crncy_code</t>
+          <t>foreign_ccy_pur_event_id</t>
         </is>
       </c>
       <c r="IY1" s="1" t="inlineStr">
         <is>
-          <t>fi_payment_tran_event_id</t>
+          <t>future_int_for_tds_elgbl</t>
         </is>
       </c>
       <c r="IZ1" s="1" t="inlineStr">
         <is>
-          <t>foreign_ccy_pur_event_id</t>
+          <t>gsv_applicable_from_date</t>
         </is>
       </c>
       <c r="JA1" s="1" t="inlineStr">
         <is>
-          <t>future_int_for_tds_elgbl</t>
+          <t>img_acc_code_for_dormant</t>
         </is>
       </c>
       <c r="JB1" s="1" t="inlineStr">
         <is>
-          <t>gsv_applicable_from_date</t>
+          <t>limit_cont_liab_tran_flg</t>
         </is>
       </c>
       <c r="JC1" s="1" t="inlineStr">
         <is>
-          <t>img_acc_code_for_dormant</t>
+          <t>loan_crncy_hol_excp_code</t>
         </is>
       </c>
       <c r="JD1" s="1" t="inlineStr">
         <is>
-          <t>limit_cont_liab_tran_flg</t>
+          <t>master_placement_enabled</t>
         </is>
       </c>
       <c r="JE1" s="1" t="inlineStr">
         <is>
-          <t>loan_crncy_hol_excp_code</t>
+          <t>non_fund_liab_reval_reqd</t>
         </is>
       </c>
       <c r="JF1" s="1" t="inlineStr">
         <is>
-          <t>master_placement_enabled</t>
+          <t>num_of_back_days_allowed</t>
         </is>
       </c>
       <c r="JG1" s="1" t="inlineStr">
         <is>
-          <t>non_fund_liab_reval_reqd</t>
+          <t>num_of_tod_alwd_for_cust</t>
         </is>
       </c>
       <c r="JH1" s="1" t="inlineStr">
         <is>
-          <t>num_of_back_days_allowed</t>
+          <t>part_recov_chrg_alwd_flg</t>
         </is>
       </c>
       <c r="JI1" s="1" t="inlineStr">
         <is>
-          <t>num_of_tod_alwd_for_cust</t>
+          <t>pdcop_coll_cont_cr_bacid</t>
         </is>
       </c>
       <c r="JJ1" s="1" t="inlineStr">
         <is>
-          <t>part_recov_chrg_alwd_flg</t>
+          <t>pdcop_coll_cont_dr_bacid</t>
         </is>
       </c>
       <c r="JK1" s="1" t="inlineStr">
         <is>
-          <t>pdcop_coll_cont_cr_bacid</t>
+          <t>percolation_required_flg</t>
         </is>
       </c>
       <c r="JL1" s="1" t="inlineStr">
         <is>
-          <t>pdcop_coll_cont_dr_bacid</t>
+          <t>raise_sales_trigger_excp</t>
         </is>
       </c>
       <c r="JM1" s="1" t="inlineStr">
         <is>
-          <t>percolation_required_flg</t>
+          <t>referral_escalation_time</t>
         </is>
       </c>
       <c r="JN1" s="1" t="inlineStr">
         <is>
-          <t>raise_sales_trigger_excp</t>
+          <t>rev_loan_trans_excp_code</t>
         </is>
       </c>
       <c r="JO1" s="1" t="inlineStr">
         <is>
-          <t>referral_escalation_time</t>
+          <t>sol_submission_mandatory</t>
         </is>
       </c>
       <c r="JP1" s="1" t="inlineStr">
         <is>
-          <t>rev_loan_trans_excp_code</t>
+          <t>tdall_not_prnt_excp_code</t>
         </is>
       </c>
       <c r="JQ1" s="1" t="inlineStr">
         <is>
-          <t>sol_submission_mandatory</t>
+          <t>undesp_atm_anw_excp_code</t>
         </is>
       </c>
       <c r="JR1" s="1" t="inlineStr">
         <is>
-          <t>tdall_not_prnt_excp_code</t>
+          <t>wrkcls_vrfy_chk_reqd_flg</t>
         </is>
       </c>
       <c r="JS1" s="1" t="inlineStr">
         <is>
-          <t>undesp_atm_anw_excp_code</t>
+          <t>ac_bal_not_zero_excp_code</t>
         </is>
       </c>
       <c r="JT1" s="1" t="inlineStr">
         <is>
-          <t>wrkcls_vrfy_chk_reqd_flg</t>
+          <t>anw_trn_incmplt_excp_code</t>
         </is>
       </c>
       <c r="JU1" s="1" t="inlineStr">
         <is>
-          <t>ac_bal_not_zero_excp_code</t>
+          <t>cd_limit_exceed_excp_code</t>
         </is>
       </c>
       <c r="JV1" s="1" t="inlineStr">
         <is>
-          <t>anw_trn_incmplt_excp_code</t>
+          <t>committed_limits_only_flg</t>
         </is>
       </c>
       <c r="JW1" s="1" t="inlineStr">
         <is>
-          <t>cd_limit_exceed_excp_code</t>
+          <t>distinctive_num_dupl_excp</t>
         </is>
       </c>
       <c r="JX1" s="1" t="inlineStr">
         <is>
-          <t>committed_limits_only_flg</t>
+          <t>dual_lang_implemented_flg</t>
         </is>
       </c>
       <c r="JY1" s="1" t="inlineStr">
         <is>
-          <t>distinctive_num_dupl_excp</t>
+          <t>external_sol_contra_bacid</t>
         </is>
       </c>
       <c r="JZ1" s="1" t="inlineStr">
         <is>
-          <t>dual_lang_implemented_flg</t>
+          <t>foreign_ccy_sale_event_id</t>
         </is>
       </c>
       <c r="KA1" s="1" t="inlineStr">
         <is>
-          <t>external_sol_contra_bacid</t>
+          <t>invalid_chq_chg_excp_code</t>
         </is>
       </c>
       <c r="KB1" s="1" t="inlineStr">
         <is>
-          <t>foreign_ccy_sale_event_id</t>
+          <t>invt_tran_npstd_excp_code</t>
         </is>
       </c>
       <c r="KC1" s="1" t="inlineStr">
         <is>
-          <t>invalid_chq_chg_excp_code</t>
+          <t>memopad_not_vfd_excp_code</t>
         </is>
       </c>
       <c r="KD1" s="1" t="inlineStr">
         <is>
-          <t>invt_tran_npstd_excp_code</t>
+          <t>num_of_tod_alwd_excp_code</t>
         </is>
       </c>
       <c r="KE1" s="1" t="inlineStr">
         <is>
-          <t>memopad_not_vfd_excp_code</t>
+          <t>pre_cls_int_amt_xced_excp</t>
         </is>
       </c>
       <c r="KF1" s="1" t="inlineStr">
         <is>
-          <t>num_of_tod_alwd_excp_code</t>
+          <t>slab_crncy_defination_flg</t>
         </is>
       </c>
       <c r="KG1" s="1" t="inlineStr">
         <is>
-          <t>pre_cls_int_amt_xced_excp</t>
+          <t>stl_out_clr_ins_excp_code</t>
         </is>
       </c>
       <c r="KH1" s="1" t="inlineStr">
         <is>
-          <t>slab_crncy_defination_flg</t>
+          <t>terminal_secu_enabled_flg</t>
         </is>
       </c>
       <c r="KI1" s="1" t="inlineStr">
         <is>
-          <t>stl_out_clr_ins_excp_code</t>
+          <t>zone_acct_crncy_diff_excp</t>
         </is>
       </c>
       <c r="KJ1" s="1" t="inlineStr">
         <is>
-          <t>terminal_secu_enabled_flg</t>
+          <t>bills_pend_verfn_excp_code</t>
         </is>
       </c>
       <c r="KK1" s="1" t="inlineStr">
         <is>
-          <t>zone_acct_crncy_diff_excp</t>
+          <t>cdci_max_num_msgs_per_tran</t>
         </is>
       </c>
       <c r="KL1" s="1" t="inlineStr">
         <is>
-          <t>bills_pend_verfn_excp_code</t>
+          <t>channel_pref_bef_cust_pref</t>
         </is>
       </c>
       <c r="KM1" s="1" t="inlineStr">
         <is>
-          <t>cdci_max_num_msgs_per_tran</t>
+          <t>cust_id_mismatch_excp_code</t>
         </is>
       </c>
       <c r="KN1" s="1" t="inlineStr">
         <is>
-          <t>channel_pref_bef_cust_pref</t>
+          <t>exchg_rate_chngd_excp_code</t>
         </is>
       </c>
       <c r="KO1" s="1" t="inlineStr">
         <is>
-          <t>cust_id_mismatch_excp_code</t>
+          <t>fd_inflow_include_end_date</t>
         </is>
       </c>
       <c r="KP1" s="1" t="inlineStr">
         <is>
-          <t>exchg_rate_chngd_excp_code</t>
+          <t>firc_agnst_remit_excp_code</t>
         </is>
       </c>
       <c r="KQ1" s="1" t="inlineStr">
         <is>
-          <t>fd_inflow_include_end_date</t>
+          <t>int_ptran_through_acct_flg</t>
         </is>
       </c>
       <c r="KR1" s="1" t="inlineStr">
         <is>
-          <t>firc_agnst_remit_excp_code</t>
+          <t>limxfr_across_lt_excp_code</t>
         </is>
       </c>
       <c r="KS1" s="1" t="inlineStr">
         <is>
-          <t>int_ptran_through_acct_flg</t>
+          <t>lnk_acct_to_overdrawnlimit</t>
         </is>
       </c>
       <c r="KT1" s="1" t="inlineStr">
         <is>
-          <t>limxfr_across_lt_excp_code</t>
+          <t>next_purchase_ref_nnt_code</t>
         </is>
       </c>
       <c r="KU1" s="1" t="inlineStr">
         <is>
-          <t>lnk_acct_to_overdrawnlimit</t>
+          <t>num_of_future_days_allowed</t>
         </is>
       </c>
       <c r="KV1" s="1" t="inlineStr">
         <is>
-          <t>next_purchase_ref_nnt_code</t>
+          <t>pdcop_pledge_amt_excp_code</t>
         </is>
       </c>
       <c r="KW1" s="1" t="inlineStr">
         <is>
-          <t>num_of_future_days_allowed</t>
+          <t>profit_loss_pend_excp_code</t>
         </is>
       </c>
       <c r="KX1" s="1" t="inlineStr">
         <is>
-          <t>pdcop_pledge_amt_excp_code</t>
+          <t>sanct_lim_expired_excp_flg</t>
         </is>
       </c>
       <c r="KY1" s="1" t="inlineStr">
         <is>
-          <t>profit_loss_pend_excp_code</t>
+          <t>standalone_coltrl_reqd_flg</t>
         </is>
       </c>
       <c r="KZ1" s="1" t="inlineStr">
         <is>
-          <t>sanct_lim_expired_excp_flg</t>
+          <t>syn_cond_not_met_excp_code</t>
         </is>
       </c>
       <c r="LA1" s="1" t="inlineStr">
         <is>
-          <t>standalone_coltrl_reqd_flg</t>
+          <t>td_ovdu_int_accr_book_reqd</t>
         </is>
       </c>
       <c r="LB1" s="1" t="inlineStr">
         <is>
-          <t>syn_cond_not_met_excp_code</t>
+          <t>temp_acct_at_acct_open_flg</t>
         </is>
       </c>
       <c r="LC1" s="1" t="inlineStr">
         <is>
-          <t>td_ovdu_int_accr_book_reqd</t>
+          <t>wfs_eod_excp_priority_from</t>
         </is>
       </c>
       <c r="LD1" s="1" t="inlineStr">
         <is>
-          <t>temp_acct_at_acct_open_flg</t>
+          <t>zakat_threshold_tenor_days</t>
         </is>
       </c>
       <c r="LE1" s="1" t="inlineStr">
         <is>
-          <t>wfs_eod_excp_priority_from</t>
+          <t>zakat_threshold_tenor_mths</t>
         </is>
       </c>
       <c r="LF1" s="1" t="inlineStr">
         <is>
-          <t>zakat_threshold_tenor_days</t>
+          <t>batch_reshd_allwd_after_sec</t>
         </is>
       </c>
       <c r="LG1" s="1" t="inlineStr">
         <is>
-          <t>zakat_threshold_tenor_mths</t>
+          <t>cdci_payment_reversal_bacid</t>
         </is>
       </c>
       <c r="LH1" s="1" t="inlineStr">
         <is>
-          <t>batch_reshd_allwd_after_sec</t>
+          <t>cdci_payment_reversal_solid</t>
         </is>
       </c>
       <c r="LI1" s="1" t="inlineStr">
         <is>
-          <t>cdci_payment_reversal_bacid</t>
+          <t>channel_pref_applicable_flg</t>
         </is>
       </c>
       <c r="LJ1" s="1" t="inlineStr">
         <is>
-          <t>cdci_payment_reversal_solid</t>
+          <t>clg_posted_with_unbal_batch</t>
         </is>
       </c>
       <c r="LK1" s="1" t="inlineStr">
         <is>
-          <t>channel_pref_applicable_flg</t>
+          <t>cls_chrg_not_coll_excp_code</t>
         </is>
       </c>
       <c r="LL1" s="1" t="inlineStr">
         <is>
-          <t>clg_posted_with_unbal_batch</t>
+          <t>consolidate_part_tran_bacid</t>
         </is>
       </c>
       <c r="LM1" s="1" t="inlineStr">
         <is>
-          <t>cls_chrg_not_coll_excp_code</t>
+          <t>conv_amt_mismatch_excp_code</t>
         </is>
       </c>
       <c r="LN1" s="1" t="inlineStr">
         <is>
-          <t>consolidate_part_tran_bacid</t>
+          <t>diff_decimal_for_diff_crncy</t>
         </is>
       </c>
       <c r="LO1" s="1" t="inlineStr">
         <is>
-          <t>conv_amt_mismatch_excp_code</t>
+          <t>dorm_available_for_ccod_flg</t>
         </is>
       </c>
       <c r="LP1" s="1" t="inlineStr">
         <is>
-          <t>diff_decimal_for_diff_crncy</t>
+          <t>fd_outflow_include_end_date</t>
         </is>
       </c>
       <c r="LQ1" s="1" t="inlineStr">
         <is>
-          <t>dorm_available_for_ccod_flg</t>
+          <t>last_tran_date_reversal_flg</t>
         </is>
       </c>
       <c r="LR1" s="1" t="inlineStr">
         <is>
-          <t>fd_outflow_include_end_date</t>
+          <t>mid_rate_code_multier_ratex</t>
         </is>
       </c>
       <c r="LS1" s="1" t="inlineStr">
         <is>
-          <t>last_tran_date_reversal_flg</t>
+          <t>min_loc_cal_yyyymm_modified</t>
         </is>
       </c>
       <c r="LT1" s="1" t="inlineStr">
         <is>
-          <t>mid_rate_code_multier_ratex</t>
+          <t>next_business_tran_nnt_code</t>
         </is>
       </c>
       <c r="LU1" s="1" t="inlineStr">
         <is>
-          <t>min_loc_cal_yyyymm_modified</t>
+          <t>next_master_acct_num_prefix</t>
         </is>
       </c>
       <c r="LV1" s="1" t="inlineStr">
         <is>
-          <t>next_business_tran_nnt_code</t>
+          <t>pend_busines_tran_excp_code</t>
         </is>
       </c>
       <c r="LW1" s="1" t="inlineStr">
         <is>
-          <t>next_master_acct_num_prefix</t>
+          <t>pend_vat_approval_excp_code</t>
         </is>
       </c>
       <c r="LX1" s="1" t="inlineStr">
         <is>
-          <t>pend_busines_tran_excp_code</t>
+          <t>td_full_cls_req_for_hol_mat</t>
         </is>
       </c>
       <c r="LY1" s="1" t="inlineStr">
         <is>
-          <t>pend_vat_approval_excp_code</t>
+          <t>trading_or_position_account</t>
         </is>
       </c>
       <c r="LZ1" s="1" t="inlineStr">
         <is>
-          <t>td_full_cls_req_for_hol_mat</t>
+          <t>waive_fail_charge_excp_code</t>
         </is>
       </c>
       <c r="MA1" s="1" t="inlineStr">
         <is>
-          <t>trading_or_position_account</t>
+          <t>chrgoff_nonpastdue_excp_code</t>
         </is>
       </c>
       <c r="MB1" s="1" t="inlineStr">
         <is>
-          <t>waive_fail_charge_excp_code</t>
+          <t>cs_custid_mismatch_excp_code</t>
         </is>
       </c>
       <c r="MC1" s="1" t="inlineStr">
         <is>
-          <t>chrgoff_nonpastdue_excp_code</t>
+          <t>dpd_count_from_dmd_ovdu_date</t>
         </is>
       </c>
       <c r="MD1" s="1" t="inlineStr">
         <is>
-          <t>cs_custid_mismatch_excp_code</t>
+          <t>plmnt_prior_to_mas_excp_code</t>
         </is>
       </c>
       <c r="ME1" s="1" t="inlineStr">
         <is>
-          <t>dpd_count_from_dmd_ovdu_date</t>
+          <t>swp_reltn_mismatch_excp_code</t>
         </is>
       </c>
       <c r="MF1" s="1" t="inlineStr">
         <is>
-          <t>plmnt_prior_to_mas_excp_code</t>
+          <t>syst_gen_master_acct_num_flg</t>
         </is>
       </c>
       <c r="MG1" s="1" t="inlineStr">
         <is>
-          <t>swp_reltn_mismatch_excp_code</t>
+          <t>dir_investment_weightage_pcnt</t>
         </is>
       </c>
       <c r="MH1" s="1" t="inlineStr">
         <is>
-          <t>syst_gen_master_acct_num_flg</t>
+          <t>dp_calc_against_princ_bal_flg</t>
         </is>
       </c>
       <c r="MI1" s="1" t="inlineStr">
         <is>
-          <t>dir_investment_weightage_pcnt</t>
+          <t>fail_count_for_si_autosuspend</t>
         </is>
       </c>
       <c r="MJ1" s="1" t="inlineStr">
         <is>
-          <t>dp_calc_against_princ_bal_flg</t>
+          <t>limit_act_cond_precedent_excp</t>
         </is>
       </c>
       <c r="MK1" s="1" t="inlineStr">
         <is>
-          <t>fail_count_for_si_autosuspend</t>
+          <t>nonei_intcal_include_end_date</t>
         </is>
       </c>
       <c r="ML1" s="1" t="inlineStr">
         <is>
-          <t>limit_act_cond_precedent_excp</t>
+          <t>pdc_custid_mismatch_excp_code</t>
         </is>
       </c>
       <c r="MM1" s="1" t="inlineStr">
         <is>
-          <t>nonei_intcal_include_end_date</t>
+          <t>slab_crncy_code_multier_ratex</t>
         </is>
       </c>
       <c r="MN1" s="1" t="inlineStr">
         <is>
-          <t>pdc_custid_mismatch_excp_code</t>
+          <t>syn_ddamt_excds_amt_excp_code</t>
         </is>
       </c>
       <c r="MO1" s="1" t="inlineStr">
         <is>
-          <t>slab_crncy_code_multier_ratex</t>
+          <t>syn_dflt_margin_chg_excp_code</t>
         </is>
       </c>
       <c r="MP1" s="1" t="inlineStr">
         <is>
-          <t>syn_ddamt_excds_amt_excp_code</t>
+          <t>syn_val_dt_excd_prd_excp_code</t>
         </is>
       </c>
       <c r="MQ1" s="1" t="inlineStr">
         <is>
-          <t>syn_dflt_margin_chg_excp_code</t>
+          <t>tr_cust_rate_differ_excp_code</t>
         </is>
       </c>
       <c r="MR1" s="1" t="inlineStr">
         <is>
-          <t>syn_val_dt_excd_prd_excp_code</t>
+          <t>allow_trn_aft_acccls_excp_code</t>
         </is>
       </c>
       <c r="MS1" s="1" t="inlineStr">
         <is>
-          <t>tr_cust_rate_differ_excp_code</t>
+          <t>bank_level_zakat_coll_date_flg</t>
         </is>
       </c>
       <c r="MT1" s="1" t="inlineStr">
         <is>
-          <t>allow_trn_aft_acccls_excp_code</t>
+          <t>calc_dafa_lim_based_on_cr_comp</t>
         </is>
       </c>
       <c r="MU1" s="1" t="inlineStr">
         <is>
-          <t>bank_level_zakat_coll_date_flg</t>
+          <t>futdated_out_clr_ins_excp_code</t>
         </is>
       </c>
       <c r="MV1" s="1" t="inlineStr">
         <is>
-          <t>calc_dafa_lim_based_on_cr_comp</t>
+          <t>img_acc_code_for_exp_signature</t>
         </is>
       </c>
       <c r="MW1" s="1" t="inlineStr">
         <is>
-          <t>futdated_out_clr_ins_excp_code</t>
+          <t>implemented_tier_base_rate_flg</t>
         </is>
       </c>
       <c r="MX1" s="1" t="inlineStr">
         <is>
-          <t>img_acc_code_for_exp_signature</t>
+          <t>insuf_cum_policy_amt_excp_code</t>
         </is>
       </c>
       <c r="MY1" s="1" t="inlineStr">
         <is>
-          <t>implemented_tier_base_rate_flg</t>
+          <t>num_of_days_allwd_for_tran_rev</t>
         </is>
       </c>
       <c r="MZ1" s="1" t="inlineStr">
         <is>
-          <t>insuf_cum_policy_amt_excp_code</t>
+          <t>td_discount_int_for_flow_shift</t>
         </is>
       </c>
       <c r="NA1" s="1" t="inlineStr">
         <is>
-          <t>num_of_days_allwd_for_tran_rev</t>
+          <t>tran_to_external_sol_acct_excp</t>
         </is>
       </c>
       <c r="NB1" s="1" t="inlineStr">
         <is>
-          <t>td_discount_int_for_flow_shift</t>
+          <t>treat_prin_int_sep_for_chrgoff</t>
         </is>
       </c>
       <c r="NC1" s="1" t="inlineStr">
         <is>
-          <t>tran_to_external_sol_acct_excp</t>
+          <t>trea_ref_not_entered_excp_code</t>
         </is>
       </c>
       <c r="ND1" s="1" t="inlineStr">
-        <is>
-          <t>treat_prin_int_sep_for_chrgoff</t>
-        </is>
-      </c>
-      <c r="NE1" s="1" t="inlineStr">
-        <is>
-          <t>trea_ref_not_entered_excp_code</t>
-        </is>
-      </c>
-      <c r="NF1" s="1" t="inlineStr">
-        <is>
-          <t>_airbyte_additional_properties</t>
-        </is>
-      </c>
-      <c r="NG1" s="1" t="inlineStr">
-        <is>
-          <t>source_file_path</t>
-        </is>
-      </c>
-      <c r="NH1" s="1" t="inlineStr">
         <is>
           <t>updated_at</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>8205151f-9627-4d8f-a3a7-efaa8fd9d48f</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>45532.40748583333</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0000000000000000</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
         <v>47973</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>DC</t>
+          <t>IBAC</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>IBAC</t>
-        </is>
+          <t>2024-08-23T21:11:48</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>18</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2024-08-23T21:11:48</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>18</v>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
           <t>REV</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>2002-07-15T15:48:20</t>
         </is>
       </c>
-      <c r="O2" t="n">
+      <c r="M2" t="n">
         <v>0</v>
       </c>
-      <c r="P2" t="n">
+      <c r="N2" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>CASHATVLT</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>NIC ASIA BANK LTD.</t>
+        </is>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>NIC ASIA BANK LTD.</t>
-        </is>
-      </c>
-      <c r="V2" t="n">
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>2024-08-23T00:00:00.000000</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="n">
+        <v>1707</v>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>DF</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="AA2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>2024-08-24T00:00:00.000000</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>GMT</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>FINADMIN</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>TBAADM</t>
+        </is>
+      </c>
+      <c r="AG2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>ACTCPUR</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>2025-07-15T00:00:00.000000</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>NCB</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>TCSALE</t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t>SEL</t>
+        </is>
+      </c>
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="n">
+        <v>9999</v>
+      </c>
+      <c r="AW2" t="inlineStr">
+        <is>
+          <t>10.2.5.10</t>
+        </is>
+      </c>
+      <c r="AX2" t="inlineStr">
+        <is>
+          <t>2024-07-16T00:00:00.000000</t>
+        </is>
+      </c>
+      <c r="AY2" t="n">
         <v>0</v>
       </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>2024-08-23T00:00:00.000000</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>1707</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>DF</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>2024-08-24T00:00:00.000000</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>GMT</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>FINADMIN</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>TBAADM</t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="AJ2" t="inlineStr">
-        <is>
-          <t>ACTCPUR</t>
-        </is>
-      </c>
-      <c r="AK2" t="inlineStr">
-        <is>
-          <t>2025-07-15T00:00:00.000000</t>
-        </is>
-      </c>
-      <c r="AL2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="AM2" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="AN2" t="inlineStr">
+      <c r="AZ2" t="inlineStr">
+        <is>
+          <t>10.2.5.10</t>
+        </is>
+      </c>
+      <c r="BA2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="BB2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="BC2" t="inlineStr">
+        <is>
+          <t>2018-11-06T00:00:00.000000</t>
+        </is>
+      </c>
+      <c r="BD2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="BE2" t="inlineStr">
+        <is>
+          <t>NP</t>
+        </is>
+      </c>
+      <c r="BF2" t="inlineStr">
+        <is>
+          <t>NPR</t>
+        </is>
+      </c>
+      <c r="BG2" t="inlineStr">
+        <is>
+          <t>NPR</t>
+        </is>
+      </c>
+      <c r="BH2" t="inlineStr"/>
+      <c r="BI2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BJ2" t="inlineStr">
         <is>
           <t>NCB</t>
         </is>
       </c>
-      <c r="AO2" t="inlineStr">
-        <is>
-          <t>TCSALE</t>
-        </is>
-      </c>
-      <c r="AP2" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="AQ2" t="inlineStr"/>
-      <c r="AR2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="AS2" t="inlineStr"/>
-      <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="inlineStr">
-        <is>
-          <t>SEL</t>
-        </is>
-      </c>
-      <c r="AV2" t="inlineStr"/>
-      <c r="AW2" t="inlineStr"/>
-      <c r="AX2" t="n">
-        <v>9999</v>
-      </c>
-      <c r="AY2" t="inlineStr">
-        <is>
-          <t>10.2.5.10</t>
-        </is>
-      </c>
-      <c r="AZ2" t="inlineStr">
-        <is>
-          <t>2024-07-16T00:00:00.000000</t>
-        </is>
-      </c>
-      <c r="BA2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB2" t="inlineStr">
-        <is>
-          <t>10.2.5.10</t>
-        </is>
-      </c>
-      <c r="BC2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="BD2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="BE2" t="inlineStr">
-        <is>
-          <t>2018-11-06T00:00:00.000000</t>
-        </is>
-      </c>
-      <c r="BF2" t="inlineStr">
+      <c r="BK2" t="inlineStr">
         <is>
           <t> </t>
         </is>
       </c>
-      <c r="BG2" t="inlineStr">
-        <is>
-          <t>NP</t>
-        </is>
-      </c>
-      <c r="BH2" t="inlineStr">
-        <is>
-          <t>NPR</t>
-        </is>
-      </c>
-      <c r="BI2" t="inlineStr">
-        <is>
-          <t>NPR</t>
-        </is>
-      </c>
-      <c r="BJ2" t="inlineStr"/>
-      <c r="BK2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="BL2" t="inlineStr">
-        <is>
-          <t>NCB</t>
-        </is>
-      </c>
+      <c r="BL2" t="inlineStr"/>
       <c r="BM2" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Y</t>
         </is>
       </c>
       <c r="BN2" t="inlineStr"/>
-      <c r="BO2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="BP2" t="inlineStr"/>
+      <c r="BO2" t="inlineStr"/>
+      <c r="BP2" t="inlineStr">
+        <is>
+          <t>PROXY</t>
+        </is>
+      </c>
       <c r="BQ2" t="inlineStr"/>
-      <c r="BR2" t="inlineStr">
-        <is>
-          <t>PROXY</t>
-        </is>
-      </c>
+      <c r="BR2" t="inlineStr"/>
       <c r="BS2" t="inlineStr"/>
       <c r="BT2" t="inlineStr"/>
       <c r="BU2" t="inlineStr"/>
-      <c r="BV2" t="inlineStr"/>
-      <c r="BW2" t="inlineStr"/>
+      <c r="BV2" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="BW2" t="inlineStr">
+        <is>
+          <t>REV</t>
+        </is>
+      </c>
       <c r="BX2" t="inlineStr">
         <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="BY2" t="inlineStr">
-        <is>
-          <t>REV</t>
-        </is>
-      </c>
-      <c r="BZ2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="BY2" t="inlineStr"/>
+      <c r="BZ2" t="inlineStr"/>
       <c r="CA2" t="inlineStr"/>
       <c r="CB2" t="inlineStr"/>
       <c r="CC2" t="inlineStr"/>
-      <c r="CD2" t="inlineStr"/>
+      <c r="CD2" t="inlineStr">
+        <is>
+          <t>10.2.5.13</t>
+        </is>
+      </c>
       <c r="CE2" t="inlineStr"/>
-      <c r="CF2" t="inlineStr">
-        <is>
-          <t>10.2.5.13</t>
-        </is>
-      </c>
-      <c r="CG2" t="inlineStr"/>
+      <c r="CF2" t="inlineStr"/>
+      <c r="CG2" t="inlineStr">
+        <is>
+          <t>NRB</t>
+        </is>
+      </c>
       <c r="CH2" t="inlineStr"/>
       <c r="CI2" t="inlineStr">
         <is>
-          <t>NRB</t>
-        </is>
-      </c>
-      <c r="CJ2" t="inlineStr"/>
-      <c r="CK2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="CJ2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="CK2" t="n">
+        <v>1</v>
       </c>
       <c r="CL2" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="CM2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="CN2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="CO2" t="n">
+      <c r="CM2" t="n">
         <v>0</v>
       </c>
-      <c r="CP2" t="n">
+      <c r="CN2" t="n">
         <v>3</v>
+      </c>
+      <c r="CO2" t="inlineStr"/>
+      <c r="CP2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
       </c>
       <c r="CQ2" t="inlineStr"/>
       <c r="CR2" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
       <c r="CS2" t="inlineStr"/>
-      <c r="CT2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="CU2" t="inlineStr"/>
+      <c r="CT2" t="inlineStr"/>
+      <c r="CU2" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
       <c r="CV2" t="inlineStr"/>
-      <c r="CW2" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
+      <c r="CW2" t="inlineStr"/>
       <c r="CX2" t="inlineStr"/>
       <c r="CY2" t="inlineStr"/>
-      <c r="CZ2" t="inlineStr"/>
+      <c r="CZ2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="DA2" t="inlineStr"/>
-      <c r="DB2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="DB2" t="inlineStr"/>
       <c r="DC2" t="inlineStr"/>
-      <c r="DD2" t="inlineStr"/>
-      <c r="DE2" t="inlineStr"/>
+      <c r="DD2" t="inlineStr">
+        <is>
+          <t>NCB</t>
+        </is>
+      </c>
+      <c r="DE2" t="inlineStr">
+        <is>
+          <t>LE2</t>
+        </is>
+      </c>
       <c r="DF2" t="inlineStr">
         <is>
-          <t>NCB</t>
-        </is>
-      </c>
-      <c r="DG2" t="inlineStr">
-        <is>
-          <t>LE2</t>
-        </is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="DG2" t="n">
+        <v>0</v>
       </c>
       <c r="DH2" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>REV</t>
         </is>
       </c>
       <c r="DI2" t="n">
@@ -2697,482 +2665,478 @@
       </c>
       <c r="DJ2" t="inlineStr">
         <is>
-          <t>REV</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="DK2" t="n">
+        <v>30</v>
+      </c>
+      <c r="DL2" t="inlineStr">
+        <is>
+          <t>NCB</t>
+        </is>
+      </c>
+      <c r="DM2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="DN2" t="n">
         <v>0</v>
       </c>
-      <c r="DL2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="DM2" t="n">
-        <v>30</v>
-      </c>
-      <c r="DN2" t="inlineStr">
-        <is>
-          <t>NCB</t>
-        </is>
-      </c>
-      <c r="DO2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="DP2" t="n">
-        <v>0</v>
-      </c>
+      <c r="DO2" t="inlineStr"/>
+      <c r="DP2" t="inlineStr"/>
       <c r="DQ2" t="inlineStr"/>
       <c r="DR2" t="inlineStr"/>
-      <c r="DS2" t="inlineStr"/>
+      <c r="DS2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="DT2" t="inlineStr"/>
-      <c r="DU2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="DU2" t="inlineStr"/>
       <c r="DV2" t="inlineStr"/>
-      <c r="DW2" t="inlineStr"/>
-      <c r="DX2" t="inlineStr"/>
-      <c r="DY2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="DZ2" t="inlineStr">
+      <c r="DW2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="DX2" t="inlineStr">
         <is>
           <t>10.2.5.13</t>
         </is>
       </c>
+      <c r="DY2" t="inlineStr"/>
+      <c r="DZ2" t="inlineStr"/>
       <c r="EA2" t="inlineStr"/>
-      <c r="EB2" t="inlineStr"/>
+      <c r="EB2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="EC2" t="inlineStr"/>
-      <c r="ED2" t="inlineStr">
+      <c r="ED2" t="n">
+        <v>999</v>
+      </c>
+      <c r="EE2" t="n">
+        <v>999</v>
+      </c>
+      <c r="EF2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="EG2" t="inlineStr">
+        <is>
+          <t>SM3</t>
+        </is>
+      </c>
+      <c r="EH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EI2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="EJ2" t="inlineStr"/>
+      <c r="EK2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="EL2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="EM2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="EN2" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="EO2" t="inlineStr"/>
+      <c r="EP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="EQ2" t="inlineStr"/>
+      <c r="ER2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="ES2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="ET2" t="inlineStr">
+        <is>
+          <t>BL2</t>
+        </is>
+      </c>
+      <c r="EU2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="EV2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="EW2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="EX2" t="inlineStr">
         <is>
           <t> </t>
         </is>
       </c>
-      <c r="EE2" t="inlineStr"/>
-      <c r="EF2" t="n">
+      <c r="EY2" t="inlineStr"/>
+      <c r="EZ2" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="FA2" t="n">
+        <v>4</v>
+      </c>
+      <c r="FB2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="FC2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="FD2" t="inlineStr">
+        <is>
+          <t>SEL</t>
+        </is>
+      </c>
+      <c r="FE2" t="n">
         <v>999</v>
       </c>
-      <c r="EG2" t="n">
-        <v>999</v>
-      </c>
-      <c r="EH2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="EI2" t="inlineStr">
-        <is>
-          <t>SM3</t>
-        </is>
-      </c>
-      <c r="EJ2" t="inlineStr">
-        <is>
-          <t>00</t>
-        </is>
-      </c>
-      <c r="EK2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="EL2" t="inlineStr"/>
-      <c r="EM2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="EN2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="EO2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="EP2" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="EQ2" t="inlineStr"/>
-      <c r="ER2" t="n">
+      <c r="FF2" t="n">
+        <v>10</v>
+      </c>
+      <c r="FG2" t="n">
         <v>0</v>
       </c>
-      <c r="ES2" t="inlineStr"/>
-      <c r="ET2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="EU2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="EV2" t="inlineStr">
-        <is>
-          <t>BL2</t>
-        </is>
-      </c>
-      <c r="EW2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="EX2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="EY2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="EZ2" t="inlineStr">
+      <c r="FH2" t="inlineStr"/>
+      <c r="FI2" t="inlineStr">
         <is>
           <t> </t>
         </is>
       </c>
-      <c r="FA2" t="inlineStr"/>
-      <c r="FB2" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
-      </c>
-      <c r="FC2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="FD2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="FE2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="FF2" t="inlineStr">
-        <is>
-          <t>SEL</t>
-        </is>
-      </c>
-      <c r="FG2" t="n">
-        <v>999</v>
-      </c>
-      <c r="FH2" t="inlineStr">
-        <is>
-          <t>010</t>
-        </is>
-      </c>
-      <c r="FI2" t="n">
+      <c r="FJ2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="FK2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="FL2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="FM2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="FN2" t="inlineStr"/>
+      <c r="FO2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="FP2" t="inlineStr">
+        <is>
+          <t>SD2</t>
+        </is>
+      </c>
+      <c r="FQ2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="FR2" t="inlineStr"/>
+      <c r="FS2" t="inlineStr">
+        <is>
+          <t>UB2</t>
+        </is>
+      </c>
+      <c r="FT2" t="inlineStr"/>
+      <c r="FU2" t="n">
         <v>0</v>
       </c>
-      <c r="FJ2" t="inlineStr"/>
-      <c r="FK2" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="FL2" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="FM2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="FN2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="FO2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="FP2" t="inlineStr"/>
-      <c r="FQ2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="FR2" t="inlineStr">
-        <is>
-          <t>SD2</t>
-        </is>
-      </c>
-      <c r="FS2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="FT2" t="inlineStr"/>
-      <c r="FU2" t="inlineStr">
-        <is>
-          <t>UB2</t>
-        </is>
-      </c>
-      <c r="FV2" t="inlineStr"/>
-      <c r="FW2" t="n">
-        <v>0</v>
+      <c r="FV2" t="inlineStr">
+        <is>
+          <t>BY3</t>
+        </is>
+      </c>
+      <c r="FW2" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
       </c>
       <c r="FX2" t="inlineStr">
         <is>
-          <t>BY3</t>
+          <t>O</t>
         </is>
       </c>
       <c r="FY2" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="FZ2" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="FZ2" t="inlineStr"/>
       <c r="GA2" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>LC2</t>
         </is>
       </c>
       <c r="GB2" t="inlineStr"/>
       <c r="GC2" t="inlineStr">
         <is>
-          <t>LC2</t>
-        </is>
-      </c>
-      <c r="GD2" t="inlineStr"/>
+          <t>CN2</t>
+        </is>
+      </c>
+      <c r="GD2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="GE2" t="inlineStr">
         <is>
-          <t>CN2</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="GF2" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>PRA</t>
         </is>
       </c>
       <c r="GG2" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
       <c r="GH2" t="inlineStr">
         <is>
-          <t>PRA</t>
-        </is>
-      </c>
-      <c r="GI2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="GI2" t="inlineStr"/>
       <c r="GJ2" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="GK2" t="inlineStr"/>
+      <c r="GK2" t="inlineStr">
+        <is>
+          <t>REV</t>
+        </is>
+      </c>
       <c r="GL2" t="inlineStr">
         <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="GM2" t="inlineStr">
-        <is>
           <t>REV</t>
         </is>
       </c>
-      <c r="GN2" t="inlineStr">
-        <is>
-          <t>REV</t>
-        </is>
+      <c r="GM2" t="inlineStr"/>
+      <c r="GN2" t="n">
+        <v>0</v>
       </c>
       <c r="GO2" t="inlineStr"/>
       <c r="GP2" t="n">
+        <v>999</v>
+      </c>
+      <c r="GQ2" t="inlineStr">
+        <is>
+          <t>SI2</t>
+        </is>
+      </c>
+      <c r="GR2" t="inlineStr">
+        <is>
+          <t>SBA,CAA,CCA,ODA,TDA</t>
+        </is>
+      </c>
+      <c r="GS2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="GT2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="GU2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="GV2" t="n">
+        <v>10</v>
+      </c>
+      <c r="GW2" t="inlineStr">
+        <is>
+          <t>REV</t>
+        </is>
+      </c>
+      <c r="GX2" t="n">
+        <v>30</v>
+      </c>
+      <c r="GY2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="GZ2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="HA2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="HB2" t="inlineStr"/>
+      <c r="HC2" t="inlineStr"/>
+      <c r="HD2" t="inlineStr"/>
+      <c r="HE2" t="inlineStr">
+        <is>
+          <t>IH3</t>
+        </is>
+      </c>
+      <c r="HF2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="HG2" t="inlineStr">
+        <is>
+          <t>UI3</t>
+        </is>
+      </c>
+      <c r="HH2" t="inlineStr">
+        <is>
+          <t>CL2</t>
+        </is>
+      </c>
+      <c r="HI2" t="n">
+        <v>99</v>
+      </c>
+      <c r="HJ2" t="n">
         <v>0</v>
-      </c>
-      <c r="GQ2" t="inlineStr"/>
-      <c r="GR2" t="n">
-        <v>999</v>
-      </c>
-      <c r="GS2" t="inlineStr">
-        <is>
-          <t>SI2</t>
-        </is>
-      </c>
-      <c r="GT2" t="inlineStr">
-        <is>
-          <t>SBA,CAA,CCA,ODA,TDA</t>
-        </is>
-      </c>
-      <c r="GU2" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="GV2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="GW2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="GX2" t="n">
-        <v>10</v>
-      </c>
-      <c r="GY2" t="inlineStr">
-        <is>
-          <t>REV</t>
-        </is>
-      </c>
-      <c r="GZ2" t="n">
-        <v>30</v>
-      </c>
-      <c r="HA2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="HB2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="HC2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="HD2" t="inlineStr"/>
-      <c r="HE2" t="inlineStr"/>
-      <c r="HF2" t="inlineStr"/>
-      <c r="HG2" t="inlineStr">
-        <is>
-          <t>IH3</t>
-        </is>
-      </c>
-      <c r="HH2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="HI2" t="inlineStr">
-        <is>
-          <t>UI3</t>
-        </is>
-      </c>
-      <c r="HJ2" t="inlineStr">
-        <is>
-          <t>CL2</t>
-        </is>
       </c>
       <c r="HK2" t="n">
         <v>99</v>
       </c>
-      <c r="HL2" t="n">
-        <v>0</v>
-      </c>
-      <c r="HM2" t="n">
-        <v>99</v>
-      </c>
-      <c r="HN2" t="inlineStr"/>
+      <c r="HL2" t="inlineStr"/>
+      <c r="HM2" t="inlineStr"/>
+      <c r="HN2" t="inlineStr">
+        <is>
+          <t>PA2</t>
+        </is>
+      </c>
       <c r="HO2" t="inlineStr"/>
       <c r="HP2" t="inlineStr">
         <is>
-          <t>PA2</t>
-        </is>
-      </c>
-      <c r="HQ2" t="inlineStr"/>
+          <t>UM3</t>
+        </is>
+      </c>
+      <c r="HQ2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="HR2" t="inlineStr">
         <is>
-          <t>UM3</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="HS2" t="inlineStr">
         <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="HT2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+          <t>TV3</t>
+        </is>
+      </c>
+      <c r="HT2" t="inlineStr"/>
       <c r="HU2" t="inlineStr">
         <is>
-          <t>TV3</t>
-        </is>
-      </c>
-      <c r="HV2" t="inlineStr"/>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="HV2" t="inlineStr">
+        <is>
+          <t>AC3</t>
+        </is>
+      </c>
       <c r="HW2" t="inlineStr">
         <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="HX2" t="inlineStr">
-        <is>
-          <t>AC3</t>
-        </is>
-      </c>
-      <c r="HY2" t="inlineStr">
-        <is>
           <t>BG3</t>
         </is>
       </c>
-      <c r="HZ2" t="n">
+      <c r="HX2" t="n">
         <v>0</v>
       </c>
-      <c r="IA2" t="inlineStr"/>
+      <c r="HY2" t="inlineStr"/>
+      <c r="HZ2" t="inlineStr">
+        <is>
+          <t>DT3</t>
+        </is>
+      </c>
+      <c r="IA2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="IB2" t="inlineStr">
         <is>
-          <t>DT3</t>
+          <t>IB3</t>
         </is>
       </c>
       <c r="IC2" t="inlineStr">
         <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="ID2" t="inlineStr">
-        <is>
-          <t>IB3</t>
-        </is>
-      </c>
-      <c r="IE2" t="inlineStr">
-        <is>
           <t>1900-01-01T00:00:00.000000</t>
         </is>
       </c>
-      <c r="IF2" t="inlineStr"/>
-      <c r="IG2" t="inlineStr"/>
+      <c r="ID2" t="inlineStr"/>
+      <c r="IE2" t="inlineStr"/>
+      <c r="IF2" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="IG2" t="inlineStr">
+        <is>
+          <t>PP3</t>
+        </is>
+      </c>
       <c r="IH2" t="inlineStr">
         <is>
-          <t>Z</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="II2" t="inlineStr">
         <is>
-          <t>PP3</t>
+          <t>N</t>
         </is>
       </c>
       <c r="IJ2" t="inlineStr">
@@ -3182,25 +3146,25 @@
       </c>
       <c r="IK2" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="IL2" t="inlineStr">
         <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="IM2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+          <t>TP3</t>
+        </is>
+      </c>
+      <c r="IM2" t="inlineStr"/>
       <c r="IN2" t="inlineStr">
         <is>
-          <t>TP3</t>
-        </is>
-      </c>
-      <c r="IO2" t="inlineStr"/>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="IO2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="IP2" t="inlineStr">
         <is>
           <t>N</t>
@@ -3208,291 +3172,289 @@
       </c>
       <c r="IQ2" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t> </t>
         </is>
       </c>
       <c r="IR2" t="inlineStr">
         <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="IS2" t="inlineStr">
+          <t>UD3</t>
+        </is>
+      </c>
+      <c r="IS2" t="inlineStr"/>
+      <c r="IT2" t="inlineStr">
+        <is>
+          <t>HL1</t>
+        </is>
+      </c>
+      <c r="IU2" t="inlineStr">
+        <is>
+          <t>DA3</t>
+        </is>
+      </c>
+      <c r="IV2" t="inlineStr">
+        <is>
+          <t>NPR</t>
+        </is>
+      </c>
+      <c r="IW2" t="inlineStr"/>
+      <c r="IX2" t="inlineStr"/>
+      <c r="IY2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="IZ2" t="inlineStr">
+        <is>
+          <t>2018-11-06T00:00:00.000000</t>
+        </is>
+      </c>
+      <c r="JA2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JB2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="JC2" t="inlineStr"/>
+      <c r="JD2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="JE2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="JF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="JG2" t="n">
+        <v>999</v>
+      </c>
+      <c r="JH2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="JI2" t="inlineStr"/>
+      <c r="JJ2" t="inlineStr"/>
+      <c r="JK2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="JL2" t="inlineStr">
+        <is>
+          <t>CV2</t>
+        </is>
+      </c>
+      <c r="JM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="JN2" t="inlineStr">
+        <is>
+          <t>LR2</t>
+        </is>
+      </c>
+      <c r="JO2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="JP2" t="inlineStr">
+        <is>
+          <t>UT2</t>
+        </is>
+      </c>
+      <c r="JQ2" t="inlineStr">
+        <is>
+          <t>UA3</t>
+        </is>
+      </c>
+      <c r="JR2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="JS2" t="inlineStr"/>
+      <c r="JT2" t="inlineStr">
+        <is>
+          <t>PN3</t>
+        </is>
+      </c>
+      <c r="JU2" t="inlineStr">
+        <is>
+          <t>DL2</t>
+        </is>
+      </c>
+      <c r="JV2" t="inlineStr">
         <is>
           <t> </t>
         </is>
       </c>
-      <c r="IT2" t="inlineStr">
-        <is>
-          <t>UD3</t>
-        </is>
-      </c>
-      <c r="IU2" t="inlineStr"/>
-      <c r="IV2" t="inlineStr">
-        <is>
-          <t>HL1</t>
-        </is>
-      </c>
-      <c r="IW2" t="inlineStr">
-        <is>
-          <t>DA3</t>
-        </is>
-      </c>
-      <c r="IX2" t="inlineStr">
-        <is>
-          <t>NPR</t>
-        </is>
-      </c>
-      <c r="IY2" t="inlineStr"/>
-      <c r="IZ2" t="inlineStr"/>
-      <c r="JA2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="JB2" t="inlineStr">
-        <is>
-          <t>2018-11-06T00:00:00.000000</t>
-        </is>
-      </c>
-      <c r="JC2" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
-      </c>
-      <c r="JD2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="JE2" t="inlineStr"/>
-      <c r="JF2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="JG2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="JH2" t="n">
-        <v>0</v>
-      </c>
-      <c r="JI2" t="n">
-        <v>999</v>
-      </c>
-      <c r="JJ2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="JK2" t="inlineStr"/>
-      <c r="JL2" t="inlineStr"/>
-      <c r="JM2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="JN2" t="inlineStr">
-        <is>
-          <t>CV2</t>
-        </is>
-      </c>
-      <c r="JO2" t="n">
-        <v>0</v>
-      </c>
-      <c r="JP2" t="inlineStr">
-        <is>
-          <t>LR2</t>
-        </is>
-      </c>
-      <c r="JQ2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="JR2" t="inlineStr">
-        <is>
-          <t>UT2</t>
-        </is>
-      </c>
-      <c r="JS2" t="inlineStr">
-        <is>
-          <t>UA3</t>
-        </is>
-      </c>
-      <c r="JT2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="JU2" t="inlineStr"/>
-      <c r="JV2" t="inlineStr">
-        <is>
-          <t>PN3</t>
-        </is>
-      </c>
       <c r="JW2" t="inlineStr">
         <is>
-          <t>DL2</t>
+          <t>DD3</t>
         </is>
       </c>
       <c r="JX2" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="JY2" t="inlineStr">
-        <is>
-          <t>DD3</t>
-        </is>
-      </c>
-      <c r="JZ2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="KA2" t="inlineStr"/>
-      <c r="KB2" t="inlineStr"/>
-      <c r="KC2" t="inlineStr">
+          <t>N</t>
+        </is>
+      </c>
+      <c r="JY2" t="inlineStr"/>
+      <c r="JZ2" t="inlineStr"/>
+      <c r="KA2" t="inlineStr">
         <is>
           <t>IC2</t>
         </is>
       </c>
-      <c r="KD2" t="inlineStr">
+      <c r="KB2" t="inlineStr">
         <is>
           <t>IT3</t>
         </is>
       </c>
-      <c r="KE2" t="inlineStr"/>
-      <c r="KF2" t="inlineStr"/>
-      <c r="KG2" t="inlineStr">
+      <c r="KC2" t="inlineStr"/>
+      <c r="KD2" t="inlineStr"/>
+      <c r="KE2" t="inlineStr">
         <is>
           <t>PC1</t>
         </is>
       </c>
+      <c r="KF2" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="KG2" t="inlineStr"/>
       <c r="KH2" t="inlineStr">
         <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="KI2" t="inlineStr"/>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="KI2" t="inlineStr">
+        <is>
+          <t>OC3</t>
+        </is>
+      </c>
       <c r="KJ2" t="inlineStr">
         <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="KK2" t="inlineStr">
-        <is>
-          <t>OC3</t>
-        </is>
+          <t>BP3</t>
+        </is>
+      </c>
+      <c r="KK2" t="n">
+        <v>300</v>
       </c>
       <c r="KL2" t="inlineStr">
         <is>
-          <t>BP3</t>
-        </is>
-      </c>
-      <c r="KM2" t="n">
-        <v>300</v>
-      </c>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="KM2" t="inlineStr"/>
       <c r="KN2" t="inlineStr">
         <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="KO2" t="inlineStr"/>
-      <c r="KP2" t="inlineStr">
-        <is>
           <t>ER2</t>
         </is>
       </c>
+      <c r="KO2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="KP2" t="inlineStr"/>
       <c r="KQ2" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
       <c r="KR2" t="inlineStr"/>
       <c r="KS2" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="KT2" t="inlineStr"/>
-      <c r="KU2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="KU2" t="n">
+        <v>7</v>
       </c>
       <c r="KV2" t="inlineStr"/>
-      <c r="KW2" t="n">
-        <v>7</v>
-      </c>
-      <c r="KX2" t="inlineStr"/>
+      <c r="KW2" t="inlineStr">
+        <is>
+          <t>PP3</t>
+        </is>
+      </c>
+      <c r="KX2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="KY2" t="inlineStr">
         <is>
-          <t>PP3</t>
-        </is>
-      </c>
-      <c r="KZ2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="KZ2" t="inlineStr"/>
       <c r="LA2" t="inlineStr">
         <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="LB2" t="inlineStr"/>
-      <c r="LC2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="LD2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="LB2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="LC2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LD2" t="n">
+        <v>0</v>
       </c>
       <c r="LE2" t="n">
-        <v>1</v>
-      </c>
-      <c r="LF2" t="n">
         <v>0</v>
       </c>
-      <c r="LG2" t="n">
-        <v>0</v>
-      </c>
-      <c r="LH2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="LI2" t="inlineStr"/>
-      <c r="LJ2" t="inlineStr"/>
+      <c r="LF2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="LG2" t="inlineStr"/>
+      <c r="LH2" t="inlineStr"/>
+      <c r="LI2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="LJ2" t="inlineStr">
+        <is>
+          <t>CP3</t>
+        </is>
+      </c>
       <c r="LK2" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>AP2</t>
         </is>
       </c>
       <c r="LL2" t="inlineStr">
         <is>
-          <t>CP3</t>
+          <t>IDVOUCHER</t>
         </is>
       </c>
       <c r="LM2" t="inlineStr">
         <is>
-          <t>AP2</t>
+          <t>CA2</t>
         </is>
       </c>
       <c r="LN2" t="inlineStr">
         <is>
-          <t>IDVOUCHER</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="LO2" t="inlineStr">
         <is>
-          <t>CA2</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="LP2" t="inlineStr">
@@ -3502,114 +3464,114 @@
       </c>
       <c r="LQ2" t="inlineStr">
         <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="LR2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="LS2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="LR2" t="inlineStr"/>
+      <c r="LS2" t="inlineStr"/>
       <c r="LT2" t="inlineStr"/>
       <c r="LU2" t="inlineStr"/>
-      <c r="LV2" t="inlineStr"/>
-      <c r="LW2" t="inlineStr"/>
+      <c r="LV2" t="inlineStr">
+        <is>
+          <t>BT3</t>
+        </is>
+      </c>
+      <c r="LW2" t="inlineStr">
+        <is>
+          <t>PV3</t>
+        </is>
+      </c>
       <c r="LX2" t="inlineStr">
         <is>
-          <t>BT3</t>
+          <t>N</t>
         </is>
       </c>
       <c r="LY2" t="inlineStr">
         <is>
-          <t>PV3</t>
-        </is>
-      </c>
-      <c r="LZ2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="MA2" t="inlineStr">
-        <is>
           <t> </t>
         </is>
       </c>
-      <c r="MB2" t="inlineStr"/>
-      <c r="MC2" t="inlineStr"/>
-      <c r="MD2" t="inlineStr">
+      <c r="LZ2" t="inlineStr"/>
+      <c r="MA2" t="inlineStr"/>
+      <c r="MB2" t="inlineStr">
         <is>
           <t>CS2</t>
         </is>
       </c>
+      <c r="MC2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="MD2" t="inlineStr"/>
       <c r="ME2" t="inlineStr">
         <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="MF2" t="inlineStr"/>
-      <c r="MG2" t="inlineStr">
-        <is>
           <t>SR3</t>
         </is>
       </c>
+      <c r="MF2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="MG2" t="n">
+        <v>100</v>
+      </c>
       <c r="MH2" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>P</t>
         </is>
       </c>
       <c r="MI2" t="n">
-        <v>100</v>
-      </c>
-      <c r="MJ2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="MK2" t="n">
         <v>0</v>
       </c>
+      <c r="MJ2" t="inlineStr"/>
+      <c r="MK2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="ML2" t="inlineStr"/>
-      <c r="MM2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
+      <c r="MM2" t="inlineStr"/>
       <c r="MN2" t="inlineStr"/>
       <c r="MO2" t="inlineStr"/>
       <c r="MP2" t="inlineStr"/>
       <c r="MQ2" t="inlineStr"/>
       <c r="MR2" t="inlineStr"/>
-      <c r="MS2" t="inlineStr"/>
-      <c r="MT2" t="inlineStr"/>
-      <c r="MU2" t="inlineStr">
+      <c r="MS2" t="inlineStr">
         <is>
           <t> </t>
         </is>
       </c>
-      <c r="MV2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="MW2" t="inlineStr"/>
-      <c r="MX2" t="inlineStr"/>
-      <c r="MY2" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
+      <c r="MT2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="MU2" t="inlineStr"/>
+      <c r="MV2" t="inlineStr"/>
+      <c r="MW2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="MX2" t="inlineStr">
+        <is>
+          <t>SU2</t>
+        </is>
+      </c>
+      <c r="MY2" t="n">
+        <v>0</v>
       </c>
       <c r="MZ2" t="inlineStr">
         <is>
-          <t>SU2</t>
-        </is>
-      </c>
-      <c r="NA2" t="n">
-        <v>0</v>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="NA2" t="inlineStr">
+        <is>
+          <t>TE1</t>
+        </is>
       </c>
       <c r="NB2" t="inlineStr">
         <is>
@@ -3618,27 +3580,11 @@
       </c>
       <c r="NC2" t="inlineStr">
         <is>
-          <t>TE1</t>
-        </is>
-      </c>
-      <c r="ND2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="NE2" t="inlineStr">
-        <is>
           <t>TR3</t>
         </is>
       </c>
-      <c r="NF2" t="inlineStr"/>
-      <c r="NG2" t="inlineStr">
-        <is>
-          <t>s3a://ai360nica/data/bronze/oracle/cbs/TBAADM/SOL_GROUP_CONTROL_TABLE/2024_08_28_1724838405696_0.parquet</t>
-        </is>
-      </c>
-      <c r="NH2" s="2" t="n">
-        <v>45533.22997499001</v>
+      <c r="ND2" s="2" t="n">
+        <v>45533.22997498843</v>
       </c>
     </row>
   </sheetData>

</xml_diff>